<commit_message>
fix alternate material cookbook failing with the addition of days_unit parameter
</commit_message>
<xml_diff>
--- a/doc/examples/buffer/alternate-materials.xlsx
+++ b/doc/examples/buffer/alternate-materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\community\doc\user-guide\cookbook\buffer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\frepple-enterprise\doc\examples\buffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2708D919-B601-443C-A3F5-7B9A5B062BF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E44244-BE4E-4202-A922-41BDB3FA6ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>Determines whether confirmed manufacturing orders consume material or not. Default is true.</t>
+  </si>
+  <si>
+    <t>days_unit</t>
+  </si>
+  <si>
+    <t>Determines whether numbers in spreadsheets are considered as days or seconds. Default is true (for days).</t>
   </si>
 </sst>
 </file>
@@ -771,10 +777,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -932,6 +938,17 @@
       </c>
       <c r="C14" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1232,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1255,7 +1272,7 @@
         <v>29</v>
       </c>
       <c r="D2">
-        <v>864000</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1272,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="D3">
-        <v>864000</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1289,7 +1306,7 @@
         <v>29</v>
       </c>
       <c r="D4">
-        <v>864000</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1306,7 +1323,7 @@
         <v>29</v>
       </c>
       <c r="D5">
-        <v>6048000</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1323,7 +1340,7 @@
         <v>29</v>
       </c>
       <c r="D6">
-        <v>864000</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1339,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1411,7 +1428,7 @@
         <v>39</v>
       </c>
       <c r="I2">
-        <v>86400</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1437,7 +1454,7 @@
         <v>39</v>
       </c>
       <c r="I3">
-        <v>86400</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update examples for changed parameter name
</commit_message>
<xml_diff>
--- a/doc/examples/buffer/alternate-materials.xlsx
+++ b/doc/examples/buffer/alternate-materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\frepple-enterprise\doc\examples\buffer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-enterprise\doc\examples\buffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E44244-BE4E-4202-A922-41BDB3FA6ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD91A2DC-C411-4643-9668-34C973F1C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="731" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -280,10 +280,10 @@
     <t>Determines whether confirmed manufacturing orders consume material or not. Default is true.</t>
   </si>
   <si>
-    <t>days_unit</t>
-  </si>
-  <si>
     <t>Determines whether numbers in spreadsheets are considered as days or seconds. Default is true (for days).</t>
+  </si>
+  <si>
+    <t>excel_duration_in_days</t>
   </si>
 </sst>
 </file>
@@ -293,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,7 +645,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -654,7 +654,7 @@
     <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -700,7 +700,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -723,7 +723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -746,7 +746,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -779,17 +779,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -811,7 +811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -822,7 +822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -833,7 +833,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -844,7 +844,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -855,7 +855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -866,7 +866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -874,7 +874,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -885,7 +885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -896,7 +896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -907,7 +907,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -918,7 +918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -929,7 +929,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -940,15 +940,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -965,14 +965,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -983,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1056,14 +1056,14 @@
       <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1082,17 +1082,17 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1111,14 +1111,14 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1209,14 +1209,14 @@
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1235,7 +1235,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -1244,7 +1244,7 @@
     <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1356,11 +1356,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -1373,7 +1373,7 @@
     <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1471,7 +1471,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -1482,7 +1482,7 @@
     <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>

</xml_diff>